<commit_message>
graph stack code added
</commit_message>
<xml_diff>
--- a/cucumber-testng-bdd/src/test/resources/testData/testData.xlsx
+++ b/cucumber-testng-bdd/src/test/resources/testData/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhuve\Downloads\cucumber-testng-bdd\cucumber-testng-bdd\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhuve\git\DS-ALGO-PROJECT\cucumber-testng-bdd\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A960EE-F06D-4F19-812F-278318C74DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FDB2BB-4BC5-4DAB-B5DE-54AF68D946F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -318,7 +318,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -326,7 +326,7 @@
     <col min="1" max="1" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -337,7 +337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>